<commit_message>
Copy of 00_MATLAB_Code directory into GitHub
updating all GitHub files to match what is currently in our main directory.
</commit_message>
<xml_diff>
--- a/01_MP_values/soccer/MP032_Transform.xlsx
+++ b/01_MP_values/soccer/MP032_Transform.xlsx
@@ -2,26 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\medctr\dfs\cib$\hits\Soccer\01_Player_Data_Video\2018_Fall\05_Player_Images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\medctr\dfs\cib$\shared\02_projects\mouthpiece_data_collection\00_MATLAB_Code\01_MP_values\soccer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21465" windowHeight="9090"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="24270" windowHeight="13800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" refMode="R1C1"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -109,7 +102,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -121,7 +114,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -168,6 +161,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -203,6 +213,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -357,12 +384,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -383,13 +409,13 @@
         <v>68.134033190263111</v>
       </c>
       <c r="B2">
-        <v>0.91306390395845405</v>
+        <v>0.93735980305625011</v>
       </c>
       <c r="C2">
-        <v>-0.38070592473083109</v>
+        <v>0.27896708354690442</v>
       </c>
       <c r="D2">
-        <v>0.14620980187042767</v>
+        <v>-0.20864794729803221</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -397,13 +423,13 @@
         <v>-11.20168507398925</v>
       </c>
       <c r="B3">
-        <v>-0.37809340977987382</v>
+        <v>0.33714882217054887</v>
       </c>
       <c r="C3">
-        <v>-0.65587916349016884</v>
+        <v>-0.57572686584418165</v>
       </c>
       <c r="D3">
-        <v>0.65335128099703332</v>
+        <v>0.74489546088981329</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -411,40 +437,16 @@
         <v>-61.436990862353014</v>
       </c>
       <c r="B4">
-        <v>-0.15283874106120923</v>
+        <v>8.7677085509040339E-2</v>
       </c>
       <c r="C4">
-        <v>-0.651832433815838</v>
+        <v>-0.76858047219700454</v>
       </c>
       <c r="D4">
-        <v>-0.74280199074621867</v>
+        <v>-0.63371664522408611</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>